<commit_message>
assignment3 correct new mem map
</commit_message>
<xml_diff>
--- a/Assignments/Assigment_3/AC_Trab_3.xlsx
+++ b/Assignments/Assigment_3/AC_Trab_3.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="76">
   <si>
     <t xml:space="preserve">FFFF</t>
   </si>
@@ -81,40 +81,37 @@
     <t xml:space="preserve">!A15 !A14</t>
   </si>
   <si>
-    <t xml:space="preserve">OUT PORT</t>
+    <t xml:space="preserve">OUT PORT (fold-back)</t>
   </si>
   <si>
     <t xml:space="preserve">0xFFFF</t>
   </si>
   <si>
-    <t xml:space="preserve">foldbak</t>
+    <t xml:space="preserve">CS = A15 A14 A13 A12  A11 A10</t>
   </si>
   <si>
     <t xml:space="preserve">0xFC00</t>
   </si>
   <si>
-    <t xml:space="preserve">cs = A15 A14 A13 A12  A11 A10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IN PORT</t>
+    <t xml:space="preserve">IN PORT(fold-back)</t>
   </si>
   <si>
     <t xml:space="preserve">0xFBFF</t>
   </si>
   <si>
+    <t xml:space="preserve">CS = A15  A14 A13 A12 A11 !A10</t>
+  </si>
+  <si>
     <t xml:space="preserve">0xF800</t>
   </si>
   <si>
-    <t xml:space="preserve">cs = A15  A14 A13 A12  A11 !A10</t>
-  </si>
-  <si>
     <t xml:space="preserve">NOT USED</t>
   </si>
   <si>
     <t xml:space="preserve">0x5FFF</t>
   </si>
   <si>
-    <t xml:space="preserve">cs = !A15 A14 !A13</t>
+    <t xml:space="preserve">CS = !A15 A14 !A13</t>
   </si>
   <si>
     <t xml:space="preserve">8K</t>
@@ -126,7 +123,7 @@
     <t xml:space="preserve">0x3FFF</t>
   </si>
   <si>
-    <t xml:space="preserve">cs = !A15 !A14</t>
+    <t xml:space="preserve">CS = !A15 !A14</t>
   </si>
   <si>
     <t xml:space="preserve">32K</t>
@@ -1706,10 +1703,15 @@
   <dimension ref="B2:J22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="30.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="1.83"/>
+  </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="33" t="s">
@@ -1719,9 +1721,10 @@
       <c r="E2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="F2" s="34" t="s">
         <v>21</v>
       </c>
+      <c r="J2" s="34"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
@@ -1729,22 +1732,21 @@
       </c>
       <c r="C3" s="33"/>
       <c r="D3" s="33"/>
-      <c r="F3" s="0" t="s">
-        <v>23</v>
-      </c>
+      <c r="F3" s="34"/>
       <c r="J3" s="34"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="35"/>
       <c r="E4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="34" t="s">
-        <v>21</v>
-      </c>
+      <c r="J4" s="34"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
@@ -1752,14 +1754,12 @@
       </c>
       <c r="C5" s="35"/>
       <c r="D5" s="35"/>
-      <c r="F5" s="0" t="s">
-        <v>27</v>
-      </c>
+      <c r="F5" s="34"/>
       <c r="J5" s="34"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="10"/>
     </row>
@@ -1783,87 +1783,100 @@
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="36" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="36"/>
       <c r="E12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="34" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="36"/>
       <c r="D13" s="36"/>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F13" s="34"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="36"/>
       <c r="D14" s="36"/>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="34"/>
+      <c r="H14" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="H14" s="0" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
-        <v>32</v>
       </c>
       <c r="C15" s="36"/>
       <c r="D15" s="36"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F15" s="34"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="37" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="37"/>
       <c r="E16" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="37"/>
       <c r="D17" s="37"/>
-    </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F17" s="34"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="37"/>
       <c r="D18" s="37"/>
-    </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F18" s="34"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="37"/>
       <c r="D19" s="37"/>
-    </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F19" s="34"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="37"/>
       <c r="D20" s="37"/>
-      <c r="F20" s="0" t="s">
+      <c r="F20" s="34"/>
+      <c r="H20" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="H20" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="37"/>
       <c r="D21" s="37"/>
-    </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F21" s="34"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="37"/>
       <c r="D22" s="37"/>
+      <c r="F22" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="11">
     <mergeCell ref="C2:D3"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="C4:D5"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="C6:D11"/>
     <mergeCell ref="C12:D15"/>
+    <mergeCell ref="F12:F15"/>
     <mergeCell ref="C16:D22"/>
+    <mergeCell ref="F16:F22"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.700694444444445" right="0.700694444444445" top="0.752083333333333" bottom="0.752083333333333" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1894,10 +1907,10 @@
   <sheetData>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="38" t="s">
         <v>37</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>38</v>
       </c>
       <c r="D2" s="38"/>
       <c r="E2" s="38"/>
@@ -1905,39 +1918,39 @@
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="38"/>
       <c r="C3" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="0" t="s">
+      <c r="G4" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1951,30 +1964,30 @@
         <v>0</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="0" t="s">
+      <c r="G6" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1988,50 +2001,50 @@
         <v>1</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="0" t="s">
+      <c r="G8" s="0" t="s">
         <v>53</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" s="0" t="s">
+      <c r="G9" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2045,30 +2058,30 @@
         <v>0</v>
       </c>
       <c r="F10" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="0" t="s">
         <v>58</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F11" s="0" t="s">
+      <c r="G11" s="0" t="s">
         <v>61</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2082,30 +2095,30 @@
         <v>1</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" s="0" t="s">
+      <c r="G13" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2119,63 +2132,63 @@
         <v>1</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F15" s="0" t="s">
+      <c r="G15" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="F16" s="0" t="s">
-        <v>72</v>
-      </c>
       <c r="G16" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="0" t="s">
         <v>73</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G18" s="0" t="s">
         <v>75</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>